<commit_message>
Added Firefox, browser selection from spreadsheet.
</commit_message>
<xml_diff>
--- a/resolver.xlsx
+++ b/resolver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,9 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
-  <si>
-    <t xml:space="preserve">C:/Users/dpenn/Desktop/Projects/Resolver/QE-index.html</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+  <si>
+    <t xml:space="preserve">file:///C:/Users/dpenn/Desktop/Projects/Resolver/QE-index.html</t>
   </si>
   <si>
     <t xml:space="preserve">page_load_element</t>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">button element</t>
   </si>
   <si>
+    <t xml:space="preserve">Browser</t>
+  </si>
+  <si>
     <t xml:space="preserve">test-1-div</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
     <t xml:space="preserve">btn</t>
   </si>
   <si>
+    <t xml:space="preserve">Chrome</t>
+  </si>
+  <si>
     <t xml:space="preserve">Expected Heading 2</t>
   </si>
   <si>
@@ -118,6 +124,9 @@
     <t xml:space="preserve">ul.list-group&gt;li.list-group-item:nth-child(2)&gt;span.badge</t>
   </si>
   <si>
+    <t xml:space="preserve">Firefox</t>
+  </si>
+  <si>
     <t xml:space="preserve">Expected Drop Down Item</t>
   </si>
   <si>
@@ -149,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">.dropdown-item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz123</t>
   </si>
   <si>
     <t xml:space="preserve">button_element</t>
@@ -279,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -293,6 +305,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -335,8 +351,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -365,10 +381,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -407,31 +423,37 @@
       <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -450,10 +472,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -468,55 +490,61 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>19</v>
+      <c r="D1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8" t="n">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -535,10 +563,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -553,49 +581,55 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>40</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -614,10 +648,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -629,31 +663,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>45</v>
+      <c r="A2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -672,10 +712,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -688,37 +728,43 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>51</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -737,10 +783,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -752,31 +798,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>55</v>
+      <c r="A2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>